<commit_message>
Test fixes, various other fixes and changes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -1978,6 +1978,9 @@
       <c r="G43">
         <v>1</v>
       </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
       <c r="I43">
         <v>1</v>
       </c>
@@ -1987,8 +1990,11 @@
       <c r="K43">
         <v>256</v>
       </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
       <c r="M43" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready to start adding quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
   <si>
     <t>name</t>
   </si>
@@ -405,6 +405,48 @@
   </si>
   <si>
     <t>A grave site of a man unknown and unamed. The land here is twisted, broken and shattered. Who lies burried here?</t>
+  </si>
+  <si>
+    <t>Northren Port</t>
+  </si>
+  <si>
+    <t>Delusional Memories</t>
+  </si>
+  <si>
+    <t>A port to the north. The men and women here are hardened fighters and vetrans of the battles between the Federation and free people of the south.</t>
+  </si>
+  <si>
+    <t>Southren Port</t>
+  </si>
+  <si>
+    <t>A port of the free people in the south. They are known to trade with peoples of the Northren Port for supplies and sending goods and services back and forth. Although these days with The Federation it's harder to trade.</t>
+  </si>
+  <si>
+    <t>Federation Controlled Town</t>
+  </si>
+  <si>
+    <t>The people here are slaves to the Federation. There's the poor and the rich, there is no in between. You either work for The Federation for nothing but scraps, or you are born into a family of one who works for The Federation. Even soldiers sent to die have a higher standing then the people of this town.</t>
+  </si>
+  <si>
+    <t>Delusional Abandoned Gold Mines</t>
+  </si>
+  <si>
+    <t>These old Gold Mines hold the memories of the past as haunting apperations.</t>
+  </si>
+  <si>
+    <t>Alchemy Corrupted Church</t>
+  </si>
+  <si>
+    <t>Purgatory's Lantern</t>
+  </si>
+  <si>
+    <t>A church corrupted by the magics of Alchemy. The gates of time have opened here, the judges of time step forth.</t>
+  </si>
+  <si>
+    <t>Federation City</t>
+  </si>
+  <si>
+    <t>The main city where the Federation organizes it's military plans from. No army, not even The Red Hawks have managed to breech the city because of the Alchemy that The Church practices, in conjunction with thier religious beliefs.</t>
   </si>
 </sst>
 </file>
@@ -744,7 +786,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,8 +794,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="37.705" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="447.034" bestFit="true" customWidth="true" style="0"/>
@@ -2219,6 +2261,174 @@
         <v>17</v>
       </c>
     </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>304</v>
+      </c>
+      <c r="K50">
+        <v>192</v>
+      </c>
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>304</v>
+      </c>
+      <c r="K51">
+        <v>288</v>
+      </c>
+      <c r="M51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>6</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+      <c r="K52">
+        <v>224</v>
+      </c>
+      <c r="M52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>6</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>448</v>
+      </c>
+      <c r="K53">
+        <v>320</v>
+      </c>
+      <c r="M53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>400</v>
+      </c>
+      <c r="K54">
+        <v>16</v>
+      </c>
+      <c r="M54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>80</v>
+      </c>
+      <c r="K55">
+        <v>96</v>
+      </c>
+      <c r="M55" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lots of minor changes, last set of quests in place for the new event map
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -398,6 +398,12 @@
     <t>These old Gold Mines hold the memories of the past as haunting apperations.</t>
   </si>
   <si>
+    <t>Abandonded Chapel</t>
+  </si>
+  <si>
+    <t>An old decrepid chapel in the middle of no where. Half burned, half rotted, what remains is a story of the past.</t>
+  </si>
+  <si>
     <t>Twisted Dimensional Gate</t>
   </si>
   <si>
@@ -437,7 +443,7 @@
     <t>Alchemy Corrupted Church</t>
   </si>
   <si>
-    <t>Purgatory's Lantern</t>
+    <t>Key to The Abandonded Church</t>
   </si>
   <si>
     <t>A church corrupted by the magics of Alchemy. The gates of time have opened here, the judges of time step forth.</t>
@@ -447,12 +453,6 @@
   </si>
   <si>
     <t>The main city where the Federation organizes it's military plans from. No army, not even The Red Hawks have managed to breech the city because of the Alchemy that The Church practices, in conjunction with thier religious beliefs.</t>
-  </si>
-  <si>
-    <t>Abandonded Chapel</t>
-  </si>
-  <si>
-    <t>An old decrepid chapel in the middle of no where. Half burned, half rotted, what remains is a story of the past.</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
     <col min="1" max="1" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="32.992" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="34.135" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="447.034" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="21.138" bestFit="true" customWidth="true" style="0"/>
@@ -2243,54 +2243,54 @@
         <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" t="s">
         <v>128</v>
       </c>
-      <c r="E49" t="s">
-        <v>129</v>
-      </c>
       <c r="G49">
         <v>1</v>
       </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
       <c r="J49">
-        <v>464</v>
+        <v>208</v>
       </c>
       <c r="K49">
-        <v>64</v>
-      </c>
-      <c r="L49">
-        <v>6</v>
+        <v>416</v>
       </c>
       <c r="M49" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
         <v>130</v>
-      </c>
-      <c r="B50" t="s">
-        <v>116</v>
       </c>
       <c r="E50" t="s">
         <v>131</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
       <c r="J50">
-        <v>288</v>
+        <v>464</v>
       </c>
       <c r="K50">
-        <v>304</v>
+        <v>64</v>
+      </c>
+      <c r="L50">
+        <v>6</v>
       </c>
       <c r="M50" t="s">
         <v>37</v>
@@ -2303,12 +2303,9 @@
       <c r="B51" t="s">
         <v>116</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>133</v>
       </c>
-      <c r="E51" t="s">
-        <v>134</v>
-      </c>
       <c r="F51">
         <v>1</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="J51">
-        <v>32</v>
+        <v>288</v>
       </c>
       <c r="K51">
         <v>304</v>
@@ -2330,10 +2327,13 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
         <v>135</v>
-      </c>
-      <c r="B52" t="s">
-        <v>123</v>
       </c>
       <c r="E52" t="s">
         <v>136</v>
@@ -2348,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="J52">
+        <v>32</v>
+      </c>
+      <c r="K52">
         <v>304</v>
-      </c>
-      <c r="K52">
-        <v>192</v>
       </c>
       <c r="M52" t="s">
         <v>37</v>
@@ -2380,7 +2380,7 @@
         <v>304</v>
       </c>
       <c r="K53">
-        <v>288</v>
+        <v>192</v>
       </c>
       <c r="M53" t="s">
         <v>37</v>
@@ -2393,23 +2393,23 @@
       <c r="B54" t="s">
         <v>123</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>140</v>
       </c>
-      <c r="E54" t="s">
-        <v>141</v>
+      <c r="F54">
+        <v>1</v>
       </c>
       <c r="G54">
         <v>1</v>
       </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
       <c r="J54">
-        <v>400</v>
+        <v>304</v>
       </c>
       <c r="K54">
-        <v>16</v>
-      </c>
-      <c r="L54">
-        <v>7</v>
+        <v>288</v>
       </c>
       <c r="M54" t="s">
         <v>37</v>
@@ -2417,11 +2417,14 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
         <v>123</v>
       </c>
+      <c r="D55" t="s">
+        <v>142</v>
+      </c>
       <c r="E55" t="s">
         <v>143</v>
       </c>
@@ -2429,10 +2432,13 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="K55">
-        <v>96</v>
+        <v>16</v>
+      </c>
+      <c r="L55">
+        <v>7</v>
       </c>
       <c r="M55" t="s">
         <v>37</v>
@@ -2442,26 +2448,23 @@
       <c r="A56" t="s">
         <v>144</v>
       </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
       <c r="E56" t="s">
         <v>145</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
-      <c r="H56">
-        <v>3</v>
-      </c>
-      <c r="I56">
-        <v>1</v>
-      </c>
       <c r="J56">
-        <v>208</v>
+        <v>80</v>
       </c>
       <c r="K56">
-        <v>416</v>
+        <v>96</v>
       </c>
       <c r="M56" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We can now move locations around the map
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -809,8 +809,8 @@
     <col min="7" max="7" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="4.57" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="4.57" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="5.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="16.425" bestFit="true" customWidth="true" style="0"/>
@@ -941,10 +941,10 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="K4">
-        <v>400</v>
+        <v>256</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
@@ -1089,10 +1089,10 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>160</v>
+        <v>480</v>
       </c>
       <c r="K9">
-        <v>80</v>
+        <v>288</v>
       </c>
       <c r="M9" t="s">
         <v>37</v>
@@ -1118,10 +1118,10 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="K10">
-        <v>496</v>
+        <v>688</v>
       </c>
       <c r="M10" t="s">
         <v>37</v>
@@ -1147,10 +1147,10 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>320</v>
+        <v>1216</v>
       </c>
       <c r="K11">
-        <v>288</v>
+        <v>768</v>
       </c>
       <c r="M11" t="s">
         <v>37</v>
@@ -1179,10 +1179,10 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>432</v>
+        <v>1264</v>
       </c>
       <c r="K12">
-        <v>208</v>
+        <v>448</v>
       </c>
       <c r="M12" t="s">
         <v>37</v>
@@ -1208,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>32</v>
+        <v>800</v>
       </c>
       <c r="K13">
-        <v>256</v>
+        <v>320</v>
       </c>
       <c r="M13" t="s">
         <v>37</v>
@@ -1234,10 +1234,10 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>320</v>
+        <v>208</v>
       </c>
       <c r="K14">
-        <v>224</v>
+        <v>624</v>
       </c>
       <c r="L14">
         <v>3</v>
@@ -1266,10 +1266,10 @@
         <v>1</v>
       </c>
       <c r="J15">
-        <v>192</v>
+        <v>592</v>
       </c>
       <c r="K15">
-        <v>176</v>
+        <v>880</v>
       </c>
       <c r="M15" t="s">
         <v>37</v>
@@ -1292,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>272</v>
+        <v>960</v>
       </c>
       <c r="K16">
-        <v>336</v>
+        <v>384</v>
       </c>
       <c r="M16" t="s">
         <v>37</v>
@@ -1321,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="K17">
-        <v>368</v>
+        <v>1216</v>
       </c>
       <c r="M17" t="s">
         <v>37</v>
@@ -1831,10 +1831,10 @@
         <v>94</v>
       </c>
       <c r="J35">
-        <v>368</v>
+        <v>1152</v>
       </c>
       <c r="K35">
-        <v>64</v>
+        <v>848</v>
       </c>
       <c r="M35" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated locations and fixed map position
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -880,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>32</v>
+        <v>416</v>
       </c>
       <c r="K2">
-        <v>400</v>
+        <v>624</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -912,10 +912,10 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>176</v>
+        <v>352</v>
       </c>
       <c r="K3">
-        <v>464</v>
+        <v>320</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>
@@ -944,7 +944,7 @@
         <v>256</v>
       </c>
       <c r="K4">
-        <v>256</v>
+        <v>304</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
@@ -970,10 +970,10 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>480</v>
+        <v>736</v>
       </c>
       <c r="K5">
-        <v>176</v>
+        <v>1232</v>
       </c>
       <c r="M5" t="s">
         <v>17</v>
@@ -999,10 +999,10 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>256</v>
+        <v>160</v>
       </c>
       <c r="K6">
-        <v>224</v>
+        <v>688</v>
       </c>
       <c r="M6" t="s">
         <v>17</v>
@@ -1028,10 +1028,10 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>208</v>
+        <v>352</v>
       </c>
       <c r="K7">
-        <v>400</v>
+        <v>672</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
@@ -1057,10 +1057,10 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>176</v>
+        <v>672</v>
       </c>
       <c r="K8">
-        <v>352</v>
+        <v>64</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1089,10 +1089,10 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>480</v>
+        <v>224</v>
       </c>
       <c r="K9">
-        <v>288</v>
+        <v>464</v>
       </c>
       <c r="M9" t="s">
         <v>37</v>
@@ -1350,10 +1350,10 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>96</v>
+        <v>576</v>
       </c>
       <c r="K18">
-        <v>240</v>
+        <v>672</v>
       </c>
       <c r="M18" t="s">
         <v>37</v>
@@ -1382,10 +1382,10 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>48</v>
+        <v>1216</v>
       </c>
       <c r="K19">
-        <v>16</v>
+        <v>448</v>
       </c>
       <c r="M19" t="s">
         <v>37</v>
@@ -1414,10 +1414,10 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>304</v>
+        <v>624</v>
       </c>
       <c r="K20">
-        <v>384</v>
+        <v>80</v>
       </c>
       <c r="M20" t="s">
         <v>37</v>
@@ -1440,10 +1440,10 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>144</v>
+        <v>480</v>
       </c>
       <c r="K21">
-        <v>432</v>
+        <v>800</v>
       </c>
       <c r="M21" t="s">
         <v>37</v>
@@ -1466,10 +1466,10 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <v>256</v>
+        <v>912</v>
       </c>
       <c r="K22">
-        <v>32</v>
+        <v>352</v>
       </c>
       <c r="M22" t="s">
         <v>37</v>
@@ -1492,10 +1492,10 @@
         <v>1</v>
       </c>
       <c r="J23">
-        <v>448</v>
+        <v>592</v>
       </c>
       <c r="K23">
-        <v>368</v>
+        <v>208</v>
       </c>
       <c r="M23" t="s">
         <v>37</v>
@@ -1521,10 +1521,10 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>464</v>
+        <v>1072</v>
       </c>
       <c r="K24">
-        <v>304</v>
+        <v>1104</v>
       </c>
       <c r="M24" t="s">
         <v>37</v>
@@ -1547,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>176</v>
+        <v>720</v>
       </c>
       <c r="K25">
-        <v>80</v>
+        <v>224</v>
       </c>
       <c r="M25" t="s">
         <v>37</v>
@@ -1576,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="J26">
-        <v>112</v>
+        <v>224</v>
       </c>
       <c r="K26">
-        <v>112</v>
+        <v>1088</v>
       </c>
       <c r="M26" t="s">
         <v>37</v>
@@ -1605,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <v>32</v>
+        <v>288</v>
       </c>
       <c r="K27">
-        <v>16</v>
+        <v>192</v>
       </c>
       <c r="M27" t="s">
         <v>37</v>
@@ -1631,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>464</v>
+        <v>880</v>
       </c>
       <c r="K28">
-        <v>336</v>
+        <v>1104</v>
       </c>
       <c r="M28" t="s">
         <v>37</v>
@@ -1660,10 +1660,10 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K29">
-        <v>144</v>
+        <v>352</v>
       </c>
       <c r="M29" t="s">
         <v>37</v>
@@ -1689,10 +1689,10 @@
         <v>1</v>
       </c>
       <c r="J30">
-        <v>80</v>
+        <v>448</v>
       </c>
       <c r="K30">
-        <v>464</v>
+        <v>528</v>
       </c>
       <c r="M30" t="s">
         <v>37</v>
@@ -1718,10 +1718,10 @@
         <v>1</v>
       </c>
       <c r="J31">
-        <v>256</v>
+        <v>704</v>
       </c>
       <c r="K31">
-        <v>336</v>
+        <v>688</v>
       </c>
       <c r="M31" t="s">
         <v>37</v>
@@ -1747,10 +1747,10 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>400</v>
+        <v>816</v>
       </c>
       <c r="K32">
-        <v>272</v>
+        <v>1120</v>
       </c>
       <c r="M32" t="s">
         <v>37</v>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <v>208</v>
+        <v>800</v>
       </c>
       <c r="K33">
         <v>64</v>
@@ -1808,10 +1808,10 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="K34">
-        <v>96</v>
+        <v>656</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -1863,10 +1863,10 @@
         <v>1</v>
       </c>
       <c r="J36">
-        <v>208</v>
+        <v>576</v>
       </c>
       <c r="K36">
-        <v>272</v>
+        <v>336</v>
       </c>
       <c r="M36" t="s">
         <v>17</v>
@@ -1895,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="J37">
-        <v>208</v>
+        <v>816</v>
       </c>
       <c r="K37">
-        <v>416</v>
+        <v>608</v>
       </c>
       <c r="M37" t="s">
         <v>17</v>
@@ -1927,10 +1927,10 @@
         <v>1</v>
       </c>
       <c r="J38">
-        <v>448</v>
+        <v>400</v>
       </c>
       <c r="K38">
-        <v>416</v>
+        <v>608</v>
       </c>
       <c r="M38" t="s">
         <v>17</v>
@@ -1959,10 +1959,10 @@
         <v>1</v>
       </c>
       <c r="J39">
-        <v>80</v>
+        <v>992</v>
       </c>
       <c r="K39">
-        <v>112</v>
+        <v>1136</v>
       </c>
       <c r="M39" t="s">
         <v>17</v>
@@ -1988,10 +1988,10 @@
         <v>1</v>
       </c>
       <c r="J40">
-        <v>304</v>
+        <v>624</v>
       </c>
       <c r="K40">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="M40" t="s">
         <v>17</v>
@@ -2017,10 +2017,10 @@
         <v>1</v>
       </c>
       <c r="J41">
-        <v>64</v>
+        <v>944</v>
       </c>
       <c r="K41">
-        <v>416</v>
+        <v>368</v>
       </c>
       <c r="M41" t="s">
         <v>17</v>
@@ -2049,10 +2049,10 @@
         <v>1</v>
       </c>
       <c r="J42">
-        <v>16</v>
+        <v>944</v>
       </c>
       <c r="K42">
-        <v>272</v>
+        <v>464</v>
       </c>
       <c r="M42" t="s">
         <v>17</v>
@@ -2078,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="J43">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="K43">
-        <v>256</v>
+        <v>784</v>
       </c>
       <c r="L43">
         <v>5</v>
@@ -2113,10 +2113,10 @@
         <v>1</v>
       </c>
       <c r="J44">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="K44">
-        <v>128</v>
+        <v>928</v>
       </c>
       <c r="M44" t="s">
         <v>17</v>
@@ -2142,10 +2142,10 @@
         <v>1</v>
       </c>
       <c r="J45">
-        <v>384</v>
+        <v>560</v>
       </c>
       <c r="K45">
-        <v>304</v>
+        <v>832</v>
       </c>
       <c r="M45" t="s">
         <v>17</v>
@@ -2171,10 +2171,10 @@
         <v>1</v>
       </c>
       <c r="J46">
-        <v>384</v>
+        <v>128</v>
       </c>
       <c r="K46">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="M46" t="s">
         <v>17</v>
@@ -2200,10 +2200,10 @@
         <v>1</v>
       </c>
       <c r="J47">
-        <v>16</v>
+        <v>224</v>
       </c>
       <c r="K47">
-        <v>224</v>
+        <v>128</v>
       </c>
       <c r="M47" t="s">
         <v>17</v>
@@ -2229,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="J48">
-        <v>448</v>
+        <v>672</v>
       </c>
       <c r="K48">
-        <v>320</v>
+        <v>480</v>
       </c>
       <c r="M48" t="s">
         <v>17</v>
@@ -2258,10 +2258,10 @@
         <v>1</v>
       </c>
       <c r="J49">
-        <v>208</v>
+        <v>1168</v>
       </c>
       <c r="K49">
-        <v>416</v>
+        <v>608</v>
       </c>
       <c r="M49" t="s">
         <v>17</v>
@@ -2284,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="J50">
-        <v>464</v>
+        <v>688</v>
       </c>
       <c r="K50">
-        <v>64</v>
+        <v>432</v>
       </c>
       <c r="L50">
         <v>6</v>
@@ -2316,10 +2316,10 @@
         <v>1</v>
       </c>
       <c r="J51">
-        <v>288</v>
+        <v>176</v>
       </c>
       <c r="K51">
-        <v>304</v>
+        <v>560</v>
       </c>
       <c r="M51" t="s">
         <v>37</v>
@@ -2348,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="J52">
-        <v>32</v>
+        <v>1152</v>
       </c>
       <c r="K52">
-        <v>304</v>
+        <v>240</v>
       </c>
       <c r="M52" t="s">
         <v>37</v>
@@ -2377,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="J53">
-        <v>304</v>
+        <v>464</v>
       </c>
       <c r="K53">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="M53" t="s">
         <v>37</v>
@@ -2406,10 +2406,10 @@
         <v>1</v>
       </c>
       <c r="J54">
-        <v>304</v>
+        <v>624</v>
       </c>
       <c r="K54">
-        <v>288</v>
+        <v>688</v>
       </c>
       <c r="M54" t="s">
         <v>37</v>
@@ -2432,10 +2432,10 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <v>400</v>
+        <v>64</v>
       </c>
       <c r="K55">
-        <v>16</v>
+        <v>496</v>
       </c>
       <c r="L55">
         <v>7</v>
@@ -2458,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <v>80</v>
+        <v>960</v>
       </c>
       <c r="K56">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M56" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated various aspects and the building upgrade section is working.
- Various fixes
- Building upgrade/repair section works
- Log fixes
- New quests
- New items
- New Monsters
- New Location
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>name</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>The main city where the Federation organizes it's military plans from. No army, not even The Red Hawks have managed to breech the city because of the Alchemy that The Church practices, in conjunction with thier religious beliefs.</t>
+  </si>
+  <si>
+    <t>Lords Stronghold</t>
+  </si>
+  <si>
+    <t>Key to the Stronghold</t>
+  </si>
+  <si>
+    <t>The Lords of the Shade Realm live with in this strong hold. Seeking nothing but total control of the past.</t>
   </si>
 </sst>
 </file>
@@ -792,7 +801,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2467,6 +2476,35 @@
         <v>37</v>
       </c>
     </row>
+    <row r="57" spans="1:14">
+      <c r="A57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" t="s">
+        <v>148</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>2112</v>
+      </c>
+      <c r="K57">
+        <v>2112</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A ton of changes, fixes and we have another raid event and main event page created.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -2279,7 +2279,7 @@
         <v>1168</v>
       </c>
       <c r="K49">
-        <v>608</v>
+        <v>752</v>
       </c>
       <c r="M49" t="s">
         <v>17</v>
@@ -2424,10 +2424,10 @@
         <v>1</v>
       </c>
       <c r="J54">
-        <v>1328</v>
+        <v>1360</v>
       </c>
       <c r="K54">
-        <v>1744</v>
+        <v>1760</v>
       </c>
       <c r="M54" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated a lot of the game and the way we schedule yearly based events.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
   <si>
     <t>name</t>
   </si>
@@ -486,6 +486,39 @@
   </si>
   <si>
     <t>An old dilapidated house where The Drunk lives i his own memories, in his own pain.</t>
+  </si>
+  <si>
+    <t>Frozen Poets House</t>
+  </si>
+  <si>
+    <t>The Poet has a house on Surface, alas this is the same house - by the same field where The Child awoke all those years ago. This house is frozen in ice, covered in memories of another time. Inhabited, not by The Poert, but another ...</t>
+  </si>
+  <si>
+    <t>Forgotten Christmas Tree Lot</t>
+  </si>
+  <si>
+    <t>A forgotten lot where christmas trees were once sold. All that stands here now is a ramshackle hut, some dead, old trees and a chain link fence that is half fallen down.</t>
+  </si>
+  <si>
+    <t>christmas-tree-x-pin</t>
+  </si>
+  <si>
+    <t>Banshee Fields of Tomorrow</t>
+  </si>
+  <si>
+    <t>Lost in these vast and forbidding fields lives a queen of the banshees. Her screams are the wind that howls around you in torment.</t>
+  </si>
+  <si>
+    <t>Frozen Pet Cemetary</t>
+  </si>
+  <si>
+    <t>A place once precious to The Creator, a place where one is burried, long ago - now forgotten and covered in the bloody snow of another time.</t>
+  </si>
+  <si>
+    <t>Ice Pirates Hideout</t>
+  </si>
+  <si>
+    <t>A port where the pirates, encased in ice live. These men and women walk around - with no soul behind their otherwise dead eyes. They sail the frozen seas searching for purpose and meaning.</t>
   </si>
 </sst>
 </file>
@@ -825,7 +858,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,7 +879,7 @@
     <col min="11" max="11" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="24.708" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2610,6 +2643,132 @@
         <v>1952</v>
       </c>
       <c r="M60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" t="s">
+        <v>158</v>
+      </c>
+      <c r="J61">
+        <v>1008</v>
+      </c>
+      <c r="K61">
+        <v>256</v>
+      </c>
+      <c r="M61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" t="s">
+        <v>160</v>
+      </c>
+      <c r="J62">
+        <v>304</v>
+      </c>
+      <c r="K62">
+        <v>1232</v>
+      </c>
+      <c r="M62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" t="s">
+        <v>96</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+      <c r="J63">
+        <v>1856</v>
+      </c>
+      <c r="K63">
+        <v>736</v>
+      </c>
+      <c r="M63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" t="s">
+        <v>165</v>
+      </c>
+      <c r="J64">
+        <v>1856</v>
+      </c>
+      <c r="K64">
+        <v>2192</v>
+      </c>
+      <c r="M64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" t="s">
+        <v>167</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>240</v>
+      </c>
+      <c r="K65">
+        <v>240</v>
+      </c>
+      <c r="M65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66" t="s">
+        <v>167</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>640</v>
+      </c>
+      <c r="K66">
+        <v>1552</v>
+      </c>
+      <c r="M66" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-added guide quests, added more quests, items and new npcs. Updated the mass importer
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -858,7 +858,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2699,6 +2699,9 @@
       <c r="E63" t="s">
         <v>163</v>
       </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
       <c r="J63">
         <v>1856</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>736</v>
       </c>
       <c r="M63" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -2719,6 +2722,9 @@
       <c r="E64" t="s">
         <v>165</v>
       </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
       <c r="J64">
         <v>1856</v>
       </c>
@@ -2726,13 +2732,16 @@
         <v>2192</v>
       </c>
       <c r="M64" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>166</v>
       </c>
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
       <c r="E65" t="s">
         <v>167</v>
       </c>
@@ -2740,35 +2749,12 @@
         <v>1</v>
       </c>
       <c r="J65">
-        <v>240</v>
+        <v>640</v>
       </c>
       <c r="K65">
-        <v>240</v>
+        <v>1552</v>
       </c>
       <c r="M65" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="A66" t="s">
-        <v>166</v>
-      </c>
-      <c r="B66" t="s">
-        <v>96</v>
-      </c>
-      <c r="E66" t="s">
-        <v>167</v>
-      </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="J66">
-        <v>640</v>
-      </c>
-      <c r="K66">
-        <v>1552</v>
-      </c>
-      <c r="M66" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated monsters, Updated locations, quests and items
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
   <si>
     <t>name</t>
   </si>
@@ -522,6 +522,21 @@
   </si>
   <si>
     <t>A port where the pirates, encased in ice live. These men and women walk around - with no soul behind their otherwise dead eyes. They sail the frozen seas searching for purpose and meaning.</t>
+  </si>
+  <si>
+    <t>Cave of Memories</t>
+  </si>
+  <si>
+    <t>Simple Brass Key</t>
+  </si>
+  <si>
+    <t>A dark, damp cave full of creatures locked away. Some say they are memories that people burry deep within them selves. Memories that twist and become monsterous</t>
+  </si>
+  <si>
+    <t>Alchemcially corrupted graveyard</t>
+  </si>
+  <si>
+    <t>A grave yard by the old church. The souls of the children who were corrupted by the churches twisted alchemical practices</t>
   </si>
 </sst>
 </file>
@@ -861,7 +876,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,7 +884,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37.705" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="38.848" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="30.564" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="34.135" bestFit="true" customWidth="true" style="0"/>
@@ -2767,6 +2782,61 @@
         <v>37</v>
       </c>
     </row>
+    <row r="66" spans="1:14">
+      <c r="A66" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" t="s">
+        <v>171</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1312</v>
+      </c>
+      <c r="K66">
+        <v>560</v>
+      </c>
+      <c r="L66">
+        <v>11</v>
+      </c>
+      <c r="M66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+      <c r="E67" t="s">
+        <v>173</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>1280</v>
+      </c>
+      <c r="K67">
+        <v>2064</v>
+      </c>
+      <c r="M67" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated information, quests, monsters, npcs and locations
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
   <si>
     <t>name</t>
   </si>
@@ -537,6 +537,15 @@
   </si>
   <si>
     <t>A grave yard by the old church. The souls of the children who were corrupted by the churches twisted alchemical practices</t>
+  </si>
+  <si>
+    <t>The Cellar</t>
+  </si>
+  <si>
+    <t>Key to the old Cellar</t>
+  </si>
+  <si>
+    <t>An old dingy, dark cellar where a man is said to be chained to a wall, a man who commited his own crimes during The Shattering</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2837,6 +2846,29 @@
         <v>37</v>
       </c>
     </row>
+    <row r="68" spans="1:14">
+      <c r="A68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" t="s">
+        <v>176</v>
+      </c>
+      <c r="J68">
+        <v>1872</v>
+      </c>
+      <c r="K68">
+        <v>816</v>
+      </c>
+      <c r="M68" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated more about how location details render.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
   <si>
     <t>name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>can_players_enter</t>
   </si>
   <si>
-    <t>enemy_strength_type</t>
+    <t>enemy_strength_increase</t>
   </si>
   <si>
     <t>can_auto_battle</t>
@@ -68,7 +68,7 @@
     <t>This old place is where the gold would come from for the port below. This place is haunted by death, critters and godly creatures the shadow plane has never seen before. it is said that beneath the surface lies a series of never ending tunnels full of fearsome creatures. Alas the gates have never been opened to get access as even The Creator has no idea how to open the gates.</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>No</t>
   </si>
   <si>
     <t>Wrecked Ship</t>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>A place where the stolen goods are smuggled in.</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Port of Kalith</t>
@@ -900,7 +897,7 @@
     <col min="5" max="5" width="447.034" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="5.856" bestFit="true" customWidth="true" style="0"/>
@@ -967,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -999,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1028,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1057,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1086,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1115,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1144,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0.35</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1188,18 +1185,18 @@
         <v>352</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1217,18 +1214,18 @@
         <v>864</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1246,21 +1243,21 @@
         <v>1584</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1278,18 +1275,18 @@
         <v>1280</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1307,18 +1304,18 @@
         <v>320</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1336,21 +1333,21 @@
         <v>3</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1365,18 +1362,18 @@
         <v>1424</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1391,21 +1388,21 @@
         <v>2224</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
         <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1420,18 +1417,18 @@
         <v>1536</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1449,21 +1446,21 @@
         <v>432</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1481,21 +1478,21 @@
         <v>176</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
       <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
         <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1513,18 +1510,18 @@
         <v>960</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1539,18 +1536,18 @@
         <v>1472</v>
       </c>
       <c r="M21" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1565,18 +1562,18 @@
         <v>464</v>
       </c>
       <c r="M22" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1591,18 +1588,18 @@
         <v>816</v>
       </c>
       <c r="M23" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1620,18 +1617,18 @@
         <v>496</v>
       </c>
       <c r="M24" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1646,18 +1643,18 @@
         <v>640</v>
       </c>
       <c r="M25" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1675,18 +1672,18 @@
         <v>416</v>
       </c>
       <c r="M26" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1704,18 +1701,18 @@
         <v>912</v>
       </c>
       <c r="M27" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1730,18 +1727,18 @@
         <v>1344</v>
       </c>
       <c r="M28" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1759,18 +1756,18 @@
         <v>560</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1788,18 +1785,18 @@
         <v>1168</v>
       </c>
       <c r="M30" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1817,18 +1814,18 @@
         <v>2032</v>
       </c>
       <c r="M31" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1846,18 +1843,18 @@
         <v>576</v>
       </c>
       <c r="M32" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1875,27 +1872,27 @@
         <v>4</v>
       </c>
       <c r="M33" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="D34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" t="s">
         <v>91</v>
       </c>
-      <c r="E34" t="s">
-        <v>92</v>
-      </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>4</v>
+        <v>0.35</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -1915,13 +1912,13 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J35">
         <v>1824</v>
@@ -1930,19 +1927,19 @@
         <v>1168</v>
       </c>
       <c r="M35" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
         <v>95</v>
       </c>
-      <c r="B36" t="s">
+      <c r="E36" t="s">
         <v>96</v>
       </c>
-      <c r="E36" t="s">
-        <v>97</v>
-      </c>
       <c r="F36">
         <v>1</v>
       </c>
@@ -1950,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>0.15</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -1967,14 +1964,14 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" t="s">
         <v>98</v>
       </c>
-      <c r="B37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" t="s">
-        <v>99</v>
-      </c>
       <c r="F37">
         <v>1</v>
       </c>
@@ -1982,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>0.15</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1999,22 +1996,22 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
         <v>100</v>
       </c>
-      <c r="B38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>101</v>
       </c>
-      <c r="E38" t="s">
-        <v>102</v>
-      </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -2031,22 +2028,22 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
         <v>103</v>
       </c>
-      <c r="B39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>104</v>
       </c>
-      <c r="E39" t="s">
-        <v>105</v>
-      </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -2063,18 +2060,15 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" t="s">
-        <v>107</v>
-      </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
@@ -2092,19 +2086,16 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" t="s">
         <v>108</v>
       </c>
-      <c r="B41" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" t="s">
-        <v>109</v>
-      </c>
       <c r="G41">
         <v>1</v>
-      </c>
-      <c r="H41">
-        <v>4</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -2121,22 +2112,22 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" t="s">
         <v>110</v>
       </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>111</v>
       </c>
-      <c r="E42" t="s">
-        <v>112</v>
-      </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -2153,25 +2144,25 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s">
         <v>113</v>
       </c>
-      <c r="B43" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" t="s">
         <v>114</v>
       </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" t="s">
-        <v>115</v>
-      </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -2191,22 +2182,19 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
         <v>116</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
         <v>117</v>
       </c>
-      <c r="E44" t="s">
-        <v>118</v>
-      </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44">
         <v>1</v>
-      </c>
-      <c r="H44">
-        <v>5</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -2223,19 +2211,16 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" t="s">
         <v>119</v>
       </c>
-      <c r="B45" t="s">
-        <v>117</v>
-      </c>
-      <c r="E45" t="s">
-        <v>120</v>
-      </c>
       <c r="G45">
         <v>1</v>
-      </c>
-      <c r="H45">
-        <v>6</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -2252,19 +2237,16 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" t="s">
         <v>121</v>
       </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="E46" t="s">
-        <v>122</v>
-      </c>
       <c r="G46">
         <v>1</v>
-      </c>
-      <c r="H46">
-        <v>5</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -2281,19 +2263,16 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
         <v>123</v>
       </c>
-      <c r="B47" t="s">
+      <c r="E47" t="s">
         <v>124</v>
       </c>
-      <c r="E47" t="s">
-        <v>125</v>
-      </c>
       <c r="G47">
         <v>1</v>
-      </c>
-      <c r="H47">
-        <v>6</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -2310,19 +2289,16 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" t="s">
         <v>126</v>
       </c>
-      <c r="B48" t="s">
-        <v>124</v>
-      </c>
-      <c r="E48" t="s">
-        <v>127</v>
-      </c>
       <c r="G48">
         <v>1</v>
-      </c>
-      <c r="H48">
-        <v>6</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -2339,19 +2315,16 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" t="s">
         <v>128</v>
       </c>
-      <c r="B49" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" t="s">
-        <v>129</v>
-      </c>
       <c r="G49">
         <v>1</v>
-      </c>
-      <c r="H49">
-        <v>3</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -2368,16 +2341,16 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
         <v>30</v>
       </c>
       <c r="D50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" t="s">
         <v>131</v>
-      </c>
-      <c r="E50" t="s">
-        <v>132</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2392,18 +2365,18 @@
         <v>6</v>
       </c>
       <c r="M50" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" t="s">
         <v>133</v>
-      </c>
-      <c r="B51" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" t="s">
-        <v>134</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2421,21 +2394,21 @@
         <v>496</v>
       </c>
       <c r="M51" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
         <v>135</v>
       </c>
-      <c r="B52" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>136</v>
-      </c>
-      <c r="E52" t="s">
-        <v>137</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2453,18 +2426,18 @@
         <v>176</v>
       </c>
       <c r="M52" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" t="s">
         <v>138</v>
-      </c>
-      <c r="B53" t="s">
-        <v>124</v>
-      </c>
-      <c r="E53" t="s">
-        <v>139</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2482,18 +2455,18 @@
         <v>512</v>
       </c>
       <c r="M53" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>123</v>
+      </c>
+      <c r="E54" t="s">
         <v>140</v>
-      </c>
-      <c r="B54" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" t="s">
-        <v>141</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2511,21 +2484,21 @@
         <v>1760</v>
       </c>
       <c r="M54" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" t="s">
         <v>142</v>
       </c>
-      <c r="B55" t="s">
-        <v>124</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>143</v>
-      </c>
-      <c r="E55" t="s">
-        <v>144</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2540,18 +2513,18 @@
         <v>7</v>
       </c>
       <c r="M55" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" t="s">
         <v>145</v>
-      </c>
-      <c r="B56" t="s">
-        <v>124</v>
-      </c>
-      <c r="E56" t="s">
-        <v>146</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2563,21 +2536,21 @@
         <v>112</v>
       </c>
       <c r="M56" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" t="s">
         <v>148</v>
-      </c>
-      <c r="E57" t="s">
-        <v>149</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -2592,21 +2565,21 @@
         <v>8</v>
       </c>
       <c r="M57" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
         <v>30</v>
       </c>
       <c r="D58" t="s">
+        <v>150</v>
+      </c>
+      <c r="E58" t="s">
         <v>151</v>
-      </c>
-      <c r="E58" t="s">
-        <v>152</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -2621,21 +2594,21 @@
         <v>9</v>
       </c>
       <c r="M58" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" t="s">
         <v>153</v>
       </c>
-      <c r="B59" t="s">
-        <v>117</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>154</v>
-      </c>
-      <c r="E59" t="s">
-        <v>155</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -2650,18 +2623,18 @@
         <v>10</v>
       </c>
       <c r="M59" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60" t="s">
         <v>156</v>
-      </c>
-      <c r="B60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E60" t="s">
-        <v>157</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2676,18 +2649,18 @@
         <v>1952</v>
       </c>
       <c r="M60" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:14">
       <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" t="s">
         <v>158</v>
-      </c>
-      <c r="B61" t="s">
-        <v>96</v>
-      </c>
-      <c r="E61" t="s">
-        <v>159</v>
       </c>
       <c r="J61">
         <v>1008</v>
@@ -2696,18 +2669,18 @@
         <v>256</v>
       </c>
       <c r="M61" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" t="s">
         <v>160</v>
-      </c>
-      <c r="B62" t="s">
-        <v>96</v>
-      </c>
-      <c r="E62" t="s">
-        <v>161</v>
       </c>
       <c r="J62">
         <v>304</v>
@@ -2716,24 +2689,21 @@
         <v>1232</v>
       </c>
       <c r="M62" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="N62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63" t="s">
         <v>163</v>
-      </c>
-      <c r="B63" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" t="s">
-        <v>164</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
       </c>
       <c r="J63">
         <v>1856</v>
@@ -2747,16 +2717,13 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="E64" t="s">
         <v>165</v>
-      </c>
-      <c r="B64" t="s">
-        <v>96</v>
-      </c>
-      <c r="E64" t="s">
-        <v>166</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
       </c>
       <c r="J64">
         <v>1856</v>
@@ -2770,13 +2737,13 @@
     </row>
     <row r="65" spans="1:14">
       <c r="A65" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" t="s">
         <v>167</v>
-      </c>
-      <c r="B65" t="s">
-        <v>96</v>
-      </c>
-      <c r="E65" t="s">
-        <v>168</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2788,21 +2755,21 @@
         <v>1552</v>
       </c>
       <c r="M65" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" t="s">
         <v>33</v>
       </c>
       <c r="D66" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" t="s">
         <v>170</v>
-      </c>
-      <c r="E66" t="s">
-        <v>171</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2817,18 +2784,18 @@
         <v>11</v>
       </c>
       <c r="M66" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" t="s">
+        <v>123</v>
+      </c>
+      <c r="E67" t="s">
         <v>172</v>
-      </c>
-      <c r="B67" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" t="s">
-        <v>173</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2843,21 +2810,21 @@
         <v>2064</v>
       </c>
       <c r="M67" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
         <v>33</v>
       </c>
       <c r="D68" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" t="s">
         <v>175</v>
-      </c>
-      <c r="E68" t="s">
-        <v>176</v>
       </c>
       <c r="J68">
         <v>1872</v>
@@ -2866,7 +2833,7 @@
         <v>816</v>
       </c>
       <c r="M68" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to location data, procifile and core header
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -1978,9 +1978,6 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37">
-        <v>0.15</v>
-      </c>
       <c r="I37">
         <v>1</v>
       </c>
@@ -2042,9 +2039,6 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="H39">
-        <v>0.3</v>
-      </c>
       <c r="I39">
         <v>1</v>
       </c>
@@ -2071,6 +2065,9 @@
       <c r="G40">
         <v>1</v>
       </c>
+      <c r="H40">
+        <v>0.15</v>
+      </c>
       <c r="I40">
         <v>1</v>
       </c>
@@ -2097,6 +2094,9 @@
       <c r="G41">
         <v>1</v>
       </c>
+      <c r="H41">
+        <v>0.15</v>
+      </c>
       <c r="I41">
         <v>1</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -2196,6 +2196,9 @@
       <c r="G44">
         <v>1</v>
       </c>
+      <c r="H44">
+        <v>0.4</v>
+      </c>
       <c r="I44">
         <v>1</v>
       </c>
@@ -2222,6 +2225,9 @@
       <c r="G45">
         <v>1</v>
       </c>
+      <c r="H45">
+        <v>0.4</v>
+      </c>
       <c r="I45">
         <v>1</v>
       </c>
@@ -2248,6 +2254,9 @@
       <c r="G46">
         <v>1</v>
       </c>
+      <c r="H46">
+        <v>0.45</v>
+      </c>
       <c r="I46">
         <v>1</v>
       </c>
@@ -2274,6 +2283,9 @@
       <c r="G47">
         <v>1</v>
       </c>
+      <c r="H47">
+        <v>0.15</v>
+      </c>
       <c r="I47">
         <v>1</v>
       </c>
@@ -2300,6 +2312,9 @@
       <c r="G48">
         <v>1</v>
       </c>
+      <c r="H48">
+        <v>0.15</v>
+      </c>
       <c r="I48">
         <v>1</v>
       </c>
@@ -2326,6 +2341,9 @@
       <c r="G49">
         <v>1</v>
       </c>
+      <c r="H49">
+        <v>0.15</v>
+      </c>
       <c r="I49">
         <v>1</v>
       </c>
@@ -2705,6 +2723,9 @@
       <c r="E63" t="s">
         <v>163</v>
       </c>
+      <c r="H63">
+        <v>0.15</v>
+      </c>
       <c r="J63">
         <v>1856</v>
       </c>
@@ -2724,6 +2745,9 @@
       </c>
       <c r="E64" t="s">
         <v>165</v>
+      </c>
+      <c r="H64">
+        <v>0.15</v>
       </c>
       <c r="J64">
         <v>1856</v>

</xml_diff>

<commit_message>
Added more quests. Added more npcs, locations and quest items.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -546,6 +546,21 @@
   </si>
   <si>
     <t>An old dingy, dark cellar where a man is said to be chained to a wall, a man who commited his own crimes during The Shattering</t>
+  </si>
+  <si>
+    <t>Emerald Mining Town</t>
+  </si>
+  <si>
+    <t>An old Dilapidated Mining town</t>
+  </si>
+  <si>
+    <t>Twisted Memorial Crypt</t>
+  </si>
+  <si>
+    <t>Twisted Memorial Crypt Key</t>
+  </si>
+  <si>
+    <t>A crypt that contains the silence of darkness that was only once illuminated by the faint sound of a childs heart beat</t>
   </si>
 </sst>
 </file>
@@ -885,7 +900,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2869,6 +2884,61 @@
         <v>37</v>
       </c>
     </row>
+    <row r="69" spans="1:14">
+      <c r="A69" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+      <c r="E69" t="s">
+        <v>178</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>6</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>2352</v>
+      </c>
+      <c r="K69">
+        <v>64</v>
+      </c>
+      <c r="M69" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" t="s">
+        <v>180</v>
+      </c>
+      <c r="E70" t="s">
+        <v>181</v>
+      </c>
+      <c r="H70">
+        <v>6</v>
+      </c>
+      <c r="J70">
+        <v>1760</v>
+      </c>
+      <c r="K70">
+        <v>384</v>
+      </c>
+      <c r="M70" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new location, quests, and quest items
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations/locations.xlsx
+++ b/resources/data-imports/Locations/locations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="186">
   <si>
     <t>name</t>
   </si>
@@ -59,6 +59,9 @@
     <t>pin_css_class</t>
   </si>
   <si>
+    <t>hours_to_drop</t>
+  </si>
+  <si>
     <t>Gold Mine</t>
   </si>
   <si>
@@ -561,6 +564,15 @@
   </si>
   <si>
     <t>A crypt that contains the silence of darkness that was only once illuminated by the faint sound of a childs heart beat</t>
+  </si>
+  <si>
+    <t>Cave of Shadows</t>
+  </si>
+  <si>
+    <t>Ever Burning Candle</t>
+  </si>
+  <si>
+    <t>A cave full of shadows of the deep, shadows of the mind, shadows of what use to be, what never was, what could have been ...</t>
   </si>
 </sst>
 </file>
@@ -900,7 +912,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -922,9 +934,10 @@
     <col min="12" max="12" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="16.425" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,16 +980,19 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -997,18 +1013,21 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1026,18 +1045,21 @@
         <v>768</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1055,18 +1077,21 @@
         <v>192</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1084,18 +1109,21 @@
         <v>1072</v>
       </c>
       <c r="M5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1113,18 +1141,21 @@
         <v>1216</v>
       </c>
       <c r="M6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1142,18 +1173,21 @@
         <v>560</v>
       </c>
       <c r="M7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1174,18 +1208,21 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1203,18 +1240,21 @@
         <v>352</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1232,18 +1272,21 @@
         <v>864</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1261,21 +1304,24 @@
         <v>1584</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1293,18 +1339,21 @@
         <v>1280</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1322,18 +1371,21 @@
         <v>320</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1351,21 +1403,24 @@
         <v>3</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1380,18 +1435,21 @@
         <v>1424</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1406,21 +1464,24 @@
         <v>2224</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1435,18 +1496,21 @@
         <v>1536</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1464,21 +1528,24 @@
         <v>432</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1496,21 +1563,24 @@
         <v>176</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1528,18 +1598,21 @@
         <v>960</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1554,18 +1627,21 @@
         <v>1472</v>
       </c>
       <c r="M21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1580,18 +1656,21 @@
         <v>464</v>
       </c>
       <c r="M22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1606,18 +1685,21 @@
         <v>816</v>
       </c>
       <c r="M23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1635,18 +1717,21 @@
         <v>496</v>
       </c>
       <c r="M24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1661,18 +1746,21 @@
         <v>640</v>
       </c>
       <c r="M25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1690,18 +1778,21 @@
         <v>416</v>
       </c>
       <c r="M26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1719,18 +1810,21 @@
         <v>912</v>
       </c>
       <c r="M27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1745,18 +1839,21 @@
         <v>1344</v>
       </c>
       <c r="M28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1774,18 +1871,21 @@
         <v>560</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1803,18 +1903,21 @@
         <v>1168</v>
       </c>
       <c r="M30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1832,18 +1935,21 @@
         <v>2032</v>
       </c>
       <c r="M31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1861,18 +1967,21 @@
         <v>576</v>
       </c>
       <c r="M32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1890,21 +1999,24 @@
         <v>4</v>
       </c>
       <c r="M33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1925,18 +2037,21 @@
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J35">
         <v>1824</v>
@@ -1945,18 +2060,21 @@
         <v>1168</v>
       </c>
       <c r="M35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1977,18 +2095,21 @@
         <v>608</v>
       </c>
       <c r="M36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2009,21 +2130,24 @@
         <v>624</v>
       </c>
       <c r="M37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -2041,21 +2165,24 @@
         <v>1184</v>
       </c>
       <c r="M38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -2073,18 +2200,21 @@
         <v>864</v>
       </c>
       <c r="M39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -2102,18 +2232,21 @@
         <v>2048</v>
       </c>
       <c r="M40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -2131,21 +2264,24 @@
         <v>112</v>
       </c>
       <c r="M41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -2163,24 +2299,27 @@
         <v>720</v>
       </c>
       <c r="M42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2201,18 +2340,21 @@
         <v>5</v>
       </c>
       <c r="M43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2233,18 +2375,21 @@
         <v>1088</v>
       </c>
       <c r="M44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2262,18 +2407,21 @@
         <v>512</v>
       </c>
       <c r="M45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2291,18 +2439,21 @@
         <v>1360</v>
       </c>
       <c r="M46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2320,18 +2471,21 @@
         <v>336</v>
       </c>
       <c r="M47" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2349,18 +2503,21 @@
         <v>1424</v>
       </c>
       <c r="M48" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2378,21 +2535,24 @@
         <v>752</v>
       </c>
       <c r="M49" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2407,18 +2567,21 @@
         <v>6</v>
       </c>
       <c r="M50" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2436,21 +2599,24 @@
         <v>496</v>
       </c>
       <c r="M51" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2468,18 +2634,21 @@
         <v>176</v>
       </c>
       <c r="M52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2497,18 +2666,21 @@
         <v>512</v>
       </c>
       <c r="M53" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E54" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2526,21 +2698,24 @@
         <v>1760</v>
       </c>
       <c r="M54" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2555,18 +2730,21 @@
         <v>7</v>
       </c>
       <c r="M55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2578,21 +2756,24 @@
         <v>112</v>
       </c>
       <c r="M56" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E57" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -2607,21 +2788,24 @@
         <v>8</v>
       </c>
       <c r="M57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E58" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -2636,21 +2820,24 @@
         <v>9</v>
       </c>
       <c r="M58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E59" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -2665,18 +2852,21 @@
         <v>10</v>
       </c>
       <c r="M59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E60" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2691,18 +2881,21 @@
         <v>1952</v>
       </c>
       <c r="M60" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J61">
         <v>1008</v>
@@ -2711,18 +2904,21 @@
         <v>256</v>
       </c>
       <c r="M61" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E62" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J62">
         <v>304</v>
@@ -2731,21 +2927,24 @@
         <v>1232</v>
       </c>
       <c r="M62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>163</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E63" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -2757,18 +2956,21 @@
         <v>736</v>
       </c>
       <c r="M63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E64" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2780,18 +2982,21 @@
         <v>2192</v>
       </c>
       <c r="M64" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E65" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2803,21 +3008,24 @@
         <v>1552</v>
       </c>
       <c r="M65" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D66" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -2832,18 +3040,21 @@
         <v>11</v>
       </c>
       <c r="M66" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E67" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2858,21 +3069,24 @@
         <v>2064</v>
       </c>
       <c r="M67" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D68" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E68" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J68">
         <v>1872</v>
@@ -2881,18 +3095,21 @@
         <v>816</v>
       </c>
       <c r="M68" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>38</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2910,21 +3127,24 @@
         <v>64</v>
       </c>
       <c r="M69" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>18</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D70" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E70" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H70">
         <v>6</v>
@@ -2936,7 +3156,42 @@
         <v>384</v>
       </c>
       <c r="M70" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" t="s">
+        <v>184</v>
+      </c>
+      <c r="E71" t="s">
+        <v>185</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>1408</v>
+      </c>
+      <c r="K71">
+        <v>640</v>
+      </c>
+      <c r="L71">
+        <v>11</v>
+      </c>
+      <c r="M71" t="s">
+        <v>38</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>